<commit_message>
Fix total counts, and add more tests
</commit_message>
<xml_diff>
--- a/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
+++ b/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="new_trials" vbProcedure="false">Sheet1!$A$1:$H$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="260">
   <si>
     <t xml:space="preserve">trials_ids</t>
   </si>
@@ -787,6 +788,24 @@
   </si>
   <si>
     <t xml:space="preserve">University of Liverpool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-000028-34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilly S.A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-000033-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bristol Myers Squibb International Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bristol Myers Squib</t>
   </si>
 </sst>
 </file>
@@ -1167,9 +1186,9 @@
   <dimension ref="A1:J65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2935,6 +2954,34 @@
       </c>
       <c r="D120" s="0" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="1037897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add an extra parent company to fixtures, for testing purposes
</commit_message>
<xml_diff>
--- a/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
+++ b/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="new_trials" vbProcedure="false">Sheet1!$A$1:$H$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="261">
   <si>
     <t xml:space="preserve">trials_ids</t>
   </si>
@@ -797,6 +798,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lilly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilly Megacorp</t>
   </si>
   <si>
     <t xml:space="preserve">2004-000033-11</t>
@@ -1185,10 +1189,10 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D121" activeCellId="0" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2967,21 +2971,35 @@
         <v>256</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B123" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B122" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>259</v>
+      <c r="C123" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="1037897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Switch focus from unreported to reported trials
Includes small refactoring and whitespace fixes
</commit_message>
<xml_diff>
--- a/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
+++ b/euctr/frontend/tests/fixtures/normalized_sponsor_names.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$120</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,10 +36,10 @@
     <t xml:space="preserve">name_of_sponsor</t>
   </si>
   <si>
-    <t xml:space="preserve">normalized_name_only</t>
-  </si>
-  <si>
     <t xml:space="preserve">normalized_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normalized_parent_name</t>
   </si>
   <si>
     <t xml:space="preserve">search_name</t>
@@ -1190,9 +1191,9 @@
   <dimension ref="A1:J65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D121" activeCellId="0" sqref="D121"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>